<commit_message>
EPBDS-9364 Support _DEFAULT_ and simple expressions in Constants
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Constants.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Constants.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D3987B-278A-4E0E-895D-FFD2740B9AF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="11685" windowWidth="19440" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Datatypes" r:id="rId1" sheetId="11"/>
-    <sheet name="Constants" r:id="rId2" sheetId="12"/>
-    <sheet name="CM" r:id="rId3" sheetId="15"/>
-    <sheet name="DT" r:id="rId4" sheetId="13"/>
-    <sheet name="SH" r:id="rId5" sheetId="14"/>
+    <sheet name="Datatypes" sheetId="11" r:id="rId1"/>
+    <sheet name="Constants" sheetId="12" r:id="rId2"/>
+    <sheet name="CM" sheetId="15" r:id="rId3"/>
+    <sheet name="DT" sheetId="13" r:id="rId4"/>
+    <sheet name="SH" sheetId="14" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_st1">#REF!</definedName>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Автор</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B8" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -43,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C8" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="B23" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{E7378384-3F54-48AE-BC9D-EE7C78A208D0}">
       <text>
         <r>
           <rPr>
@@ -71,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C23" shapeId="0">
+    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{1694FA75-640E-4B0B-B1D2-69D787BA7891}">
       <text>
         <r>
           <rPr>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="142">
   <si>
     <t>Step</t>
   </si>
@@ -170,9 +171,6 @@
     <t>D_2</t>
   </si>
   <si>
-    <t>2.5</t>
-  </si>
-  <si>
     <t>Rules Double dt1(Double val)</t>
   </si>
   <si>
@@ -182,12 +180,6 @@
     <t>Rules Double dt2(Double val)</t>
   </si>
   <si>
-    <t>=D_1</t>
-  </si>
-  <si>
-    <t>=D_2</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult sh1()</t>
   </si>
   <si>
@@ -197,9 +189,6 @@
     <t>Spreadsheet SpreadsheetResult sh2()</t>
   </si>
   <si>
-    <t>Test sh1 sh2_Test</t>
-  </si>
-  <si>
     <t>Test dt2 dt2_Test</t>
   </si>
   <si>
@@ -501,17 +490,43 @@
   </si>
   <si>
     <t>35</t>
+  </si>
+  <si>
+    <t>= 0.5 * 5</t>
+  </si>
+  <si>
+    <t>D_3</t>
+  </si>
+  <si>
+    <t>_DEFAULT_</t>
+  </si>
+  <si>
+    <t>1.52.5</t>
+  </si>
+  <si>
+    <t>Test sh2 sh2_Test</t>
+  </si>
+  <si>
+    <t>D_4</t>
+  </si>
+  <si>
+    <t>= new BigDecimal("12.35")</t>
+  </si>
+  <si>
+    <t>=D_4</t>
+  </si>
+  <si>
+    <t>=D_1 + D_3 + D_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="12">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -635,7 +650,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442" rgb="1F497D"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,115 +817,118 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="2"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
-    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="8" fontId="10" numFmtId="0" xfId="0">
+  <cellXfs count="44">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="6" fontId="6" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="7" fontId="7" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="8" fontId="8" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="9" fontId="9" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="3">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="3">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="3" fontId="2" numFmtId="0" quotePrefix="1" xfId="3">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="7" fontId="6" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="9" fillId="9" fontId="8" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="9" fontId="8" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="6" fontId="6" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="7" fontId="6" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="8" fillId="8" fontId="8" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="9" fillId="9" fontId="8" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" borderId="3" fillId="0" fontId="11" numFmtId="0" xfId="2"/>
-    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
-    <xf applyBorder="1" applyFont="1" borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="10" fontId="10" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="10" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="10" fontId="10" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="10" fontId="10" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="10" fontId="10" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="10" fontId="10" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="12" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="3">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="9" fontId="8" numFmtId="0" quotePrefix="1" xfId="2">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="20% - Accent1 10" xfId="0"/>
-    <cellStyle builtinId="0" name="Обычный" xfId="1"/>
-    <cellStyle name="Обычный 2" xfId="2"/>
-    <cellStyle name="Обычный 6" xfId="3"/>
+    <cellStyle name="20% - Accent1 10" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Обычный 6" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -936,10 +954,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -954,14 +972,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -994,9 +1012,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1048,7 +1066,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1100,7 +1118,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1153,7 +1171,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1162,13 +1180,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1178,7 +1196,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1187,7 +1205,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1196,7 +1214,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1206,12 +1224,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1242,7 +1260,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1261,7 +1279,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1273,8 +1291,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:E54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B6:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -1282,17 +1300,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="40.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:4">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="11" t="s">
@@ -1302,12 +1320,12 @@
         <v>8</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3"/>
@@ -1315,14 +1333,14 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1331,33 +1349,33 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="B20:D20"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B4:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="34" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1373,11 +1391,11 @@
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="5" t="s">
@@ -1386,23 +1404,45 @@
       <c r="C11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>26</v>
+      <c r="D11" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D17" s="5">
         <v>0.66666666666999996</v>
@@ -1410,10 +1450,10 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D18" s="5">
         <v>0.55555555557000003</v>
@@ -1421,10 +1461,10 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5">
         <v>19993</v>
@@ -1432,10 +1472,10 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5">
         <v>9847892</v>
@@ -1443,10 +1483,10 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D21" s="5" t="b">
         <v>1</v>
@@ -1454,10 +1494,10 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D22" s="5">
         <v>-128</v>
@@ -1465,24 +1505,24 @@
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -1490,7 +1530,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D25" s="5">
         <v>23423.4234</v>
@@ -1498,21 +1538,21 @@
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D27" s="5">
         <v>5345.2340000000004</v>
@@ -1520,10 +1560,10 @@
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D28" s="5">
         <v>231.31</v>
@@ -1531,10 +1571,10 @@
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D29" s="5">
         <v>4453.3419999999996</v>
@@ -1542,10 +1582,10 @@
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D30" s="5">
         <v>43393</v>
@@ -1553,10 +1593,10 @@
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D31" s="5">
         <v>42</v>
@@ -1564,10 +1604,10 @@
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D32" s="5">
         <v>42</v>
@@ -1575,10 +1615,10 @@
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D33" s="5">
         <v>3634</v>
@@ -1586,10 +1626,10 @@
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D34" s="5">
         <v>265727564</v>
@@ -1597,10 +1637,10 @@
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D35" s="5">
         <v>23</v>
@@ -1608,10 +1648,10 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D36" s="5">
         <v>432</v>
@@ -1622,29 +1662,29 @@
         <v>4</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D39" s="5">
         <v>6</v>
@@ -1652,21 +1692,21 @@
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D41" s="5">
         <v>8972342.432</v>
@@ -1674,10 +1714,10 @@
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D42" s="5">
         <v>-4234.24</v>
@@ -1685,10 +1725,10 @@
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D43" s="5">
         <v>7356</v>
@@ -1696,10 +1736,10 @@
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D44" s="5">
         <v>546245272</v>
@@ -1707,10 +1747,10 @@
     </row>
     <row r="45" spans="2:4">
       <c r="B45" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D45" s="5">
         <v>32</v>
@@ -1718,32 +1758,32 @@
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>12</v>
@@ -1755,13 +1795,13 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B16:D16"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B6:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30:C30"/>
@@ -1769,168 +1809,168 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="42.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:7">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B7" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-    </row>
-    <row ht="15.75" r="7" spans="2:7" thickBot="1">
-      <c r="B7" s="20" t="s">
+    </row>
+    <row r="8" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B8" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row ht="16.5" r="8" spans="2:7" thickBot="1" thickTop="1">
-      <c r="B8" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row ht="16.5" r="9" spans="2:7" thickBot="1" thickTop="1">
+    <row r="9" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B9" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row ht="16.5" r="10" spans="2:7" thickBot="1" thickTop="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B10" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D10" s="23">
         <v>2</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row ht="15.75" r="11" spans="2:7" thickTop="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickTop="1"/>
     <row r="12" spans="2:7">
-      <c r="B12" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-    </row>
-    <row ht="15.75" r="13" spans="2:7" thickBot="1">
+      <c r="B12" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1">
       <c r="B13" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B14" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row ht="16.5" r="14" spans="2:7" thickBot="1" thickTop="1">
-      <c r="B14" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row ht="16.5" r="15" spans="2:7" thickBot="1" thickTop="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B15" s="20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row ht="16.5" r="16" spans="2:7" thickBot="1" thickTop="1">
+    <row r="16" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B16" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D16" s="23">
         <v>2</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row ht="15.75" r="17" spans="2:5" thickTop="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" thickTop="1"/>
     <row r="18" spans="2:5">
-      <c r="B18" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-    </row>
-    <row ht="15.75" r="19" spans="2:5" thickBot="1">
+      <c r="B18" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="37"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" thickBot="1">
       <c r="B19" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B20" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row ht="16.5" r="20" spans="2:5" thickBot="1" thickTop="1">
-      <c r="B20" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row ht="16.5" r="21" spans="2:5" thickBot="1" thickTop="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B21" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
@@ -1938,51 +1978,51 @@
         <v>12</v>
       </c>
     </row>
-    <row ht="16.5" r="22" spans="2:5" thickBot="1" thickTop="1">
+    <row r="22" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B22" s="20" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row ht="16.5" r="23" spans="2:5" thickBot="1" thickTop="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B23" s="20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row ht="16.5" r="24" spans="2:5" thickBot="1" thickTop="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B24" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C30" s="32"/>
+      <c r="B30" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="36"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>23</v>
@@ -1990,7 +2030,7 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="24" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>24</v>
@@ -1998,10 +2038,10 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2011,39 +2051,39 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B30:C30"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:I47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B5:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="41.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="55.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="60.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:8">
-      <c r="B5" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" s="34"/>
-    </row>
-    <row ht="15.75" r="6" spans="2:8" thickBot="1">
+      <c r="G5" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1">
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
@@ -2057,21 +2097,21 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15.75" r="7" spans="2:8" thickTop="1">
+    <row r="7" spans="2:8" ht="15.75" thickTop="1">
       <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="40" t="s">
-        <v>131</v>
+      <c r="G7" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row ht="15.75" r="8" spans="2:8" thickBot="1">
+    <row r="8" spans="2:8" ht="15.75" thickBot="1">
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
@@ -2079,13 +2119,13 @@
         <v>18</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row ht="15.75" r="9" spans="2:8" thickTop="1">
+    <row r="9" spans="2:8" ht="15.75" thickTop="1">
       <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
@@ -2134,10 +2174,10 @@
       </c>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="34" t="s">
+      <c r="B20" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="38" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2199,7 +2239,7 @@
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C28" s="10">
         <v>3</v>
@@ -2207,18 +2247,18 @@
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C29" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="35" t="s">
-        <v>28</v>
+      <c r="B31" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:3">
@@ -2254,11 +2294,11 @@
       </c>
     </row>
     <row r="37" spans="2:3">
-      <c r="B37" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>36</v>
+      <c r="B37" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="40" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="2:3">
@@ -2282,7 +2322,7 @@
         <v>20</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:3">
@@ -2290,18 +2330,18 @@
         <v>25</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="2:3">
-      <c r="B43" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="C43" s="36"/>
+      <c r="B43" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="39"/>
     </row>
     <row r="44" spans="2:3">
       <c r="B44" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>23</v>
@@ -2309,7 +2349,7 @@
     </row>
     <row r="45" spans="2:3">
       <c r="B45" s="26" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>24</v>
@@ -2317,52 +2357,52 @@
     </row>
     <row r="46" spans="2:3">
       <c r="B46" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" s="26" t="n">
-        <v>2.0</v>
+        <v>132</v>
+      </c>
+      <c r="C46" s="26">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:3">
       <c r="B47" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="26" t="n">
-        <v>1.0</v>
+        <v>96</v>
+      </c>
+      <c r="C47" s="26">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="G5:H5"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="B6:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B6:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:3">
-      <c r="B6" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="37"/>
+      <c r="B6" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="43"/>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="12" t="s">
@@ -2389,17 +2429,17 @@
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="39"/>
+      <c r="B11" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="42"/>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:3">
@@ -2418,74 +2458,82 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="43"/>
+    </row>
     <row r="21" spans="2:3">
-      <c r="B21" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="37"/>
+      <c r="B21" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="2:3">
-      <c r="B22" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>1</v>
+      <c r="B22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="14" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>31</v>
-      </c>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="42"/>
     </row>
     <row r="26" spans="2:3">
-      <c r="B26" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="39"/>
+      <c r="B26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="11" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:3">
-      <c r="B28" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="11">
-        <v>1.5</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>25</v>
+      <c r="B28" s="11">
+        <v>12.35</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-9646 EPBDS-9364 Update a test
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Constants.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Constants.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D3987B-278A-4E0E-895D-FFD2740B9AF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B578E5-B165-48B9-B412-91AD449152E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,17 @@
     <definedName name="_st2">#REF!</definedName>
     <definedName name="_st3">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -91,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="169">
   <si>
     <t>Step</t>
   </si>
@@ -186,9 +196,6 @@
     <t>Test sh1 sh1_Test</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult sh2()</t>
-  </si>
-  <si>
     <t>Test dt2 dt2_Test</t>
   </si>
   <si>
@@ -517,13 +524,97 @@
   </si>
   <si>
     <t>=D_1 + D_3 + D_2</t>
+  </si>
+  <si>
+    <t>DAY_SECONDS</t>
+  </si>
+  <si>
+    <t>= 24 * 60 * 60</t>
+  </si>
+  <si>
+    <t>ONE_THREETH</t>
+  </si>
+  <si>
+    <t>= 1/3</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>WHITESPACE</t>
+  </si>
+  <si>
+    <t>=" "</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>_res_.$A</t>
+  </si>
+  <si>
+    <t>_res_.$B</t>
+  </si>
+  <si>
+    <t>_res_.$C</t>
+  </si>
+  <si>
+    <t>_res_.$D</t>
+  </si>
+  <si>
+    <t>_res_.$E</t>
+  </si>
+  <si>
+    <t>_res_.$F</t>
+  </si>
+  <si>
+    <t>_res_.$G</t>
+  </si>
+  <si>
+    <t>_res_.$H</t>
+  </si>
+  <si>
+    <t>86400 null</t>
+  </si>
+  <si>
+    <t>= input</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult sh2(String input)</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>= DAY_SECONDS + WHITESPACE + NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +686,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -822,7 +919,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -888,6 +985,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -914,14 +1014,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1306,11 +1409,11 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:4">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="11" t="s">
@@ -1320,12 +1423,12 @@
         <v>8</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="3"/>
@@ -1333,14 +1436,14 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1355,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B4:D48"/>
+  <dimension ref="B4:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1369,13 +1472,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="37" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1390,410 +1493,451 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="34" t="s">
+    <row r="6" spans="2:4">
+      <c r="B6" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="5" t="s">
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D14" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D15" t="s">
         <v>134</v>
       </c>
-      <c r="D12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="D13" s="30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="34" t="s">
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.66666666666999996</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.55555555557000003</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="5">
-        <v>19993</v>
-      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D20" s="5">
-        <v>9847892</v>
+        <v>0.66666666666999996</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="5" t="b">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.55555555557000003</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D22" s="5">
-        <v>-128</v>
+        <v>19993</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="D23" s="5">
+        <v>9847892</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
+      </c>
+      <c r="D24" s="5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="5" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D25" s="5">
-        <v>23423.4234</v>
+        <v>-128</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="5">
-        <v>5345.2340000000004</v>
+        <v>54</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="5" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D28" s="5">
-        <v>231.31</v>
+        <v>23423.4234</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="5">
-        <v>4453.3419999999996</v>
+        <v>58</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D30" s="5">
-        <v>43393</v>
+        <v>5345.2340000000004</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D31" s="5">
-        <v>42</v>
+        <v>231.31</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D32" s="5">
-        <v>42</v>
+        <v>4453.3419999999996</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D33" s="5">
-        <v>3634</v>
+        <v>43393</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D34" s="5">
-        <v>265727564</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D35" s="5">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D36" s="5">
-        <v>432</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="5" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
+      </c>
+      <c r="D37" s="5">
+        <v>265727564</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
+      </c>
+      <c r="D38" s="5">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D39" s="5">
-        <v>6</v>
+        <v>432</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="5" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="5">
-        <v>8972342.432</v>
+        <v>83</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D42" s="5">
-        <v>-4234.24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D43" s="5">
-        <v>7356</v>
+        <v>88</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="D44" s="5">
-        <v>546245272</v>
+        <v>8972342.432</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D45" s="5">
-        <v>32</v>
+        <v>-4234.24</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="5" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D46" s="5">
+        <v>7356</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="5" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>103</v>
+        <v>127</v>
+      </c>
+      <c r="D47" s="5">
+        <v>546245272</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="5" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1815,34 +1959,34 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:7">
-      <c r="B6" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
+      <c r="B6" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1">
       <c r="B7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="21" t="s">
         <v>108</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B8" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>1</v>
@@ -1850,127 +1994,127 @@
     </row>
     <row r="9" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B9" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B10" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>114</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>115</v>
       </c>
       <c r="D10" s="23">
         <v>2</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" thickTop="1"/>
     <row r="12" spans="2:7">
-      <c r="B12" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="37"/>
+      <c r="B12" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1">
       <c r="B13" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>108</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B14" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B15" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
     <row r="16" spans="2:7" ht="16.5" thickTop="1" thickBot="1">
       <c r="B16" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>114</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>115</v>
       </c>
       <c r="D16" s="23">
         <v>2</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="15.75" thickTop="1"/>
     <row r="18" spans="2:5">
-      <c r="B18" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
+      <c r="B18" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
     </row>
     <row r="19" spans="2:5" ht="15.75" thickBot="1">
       <c r="B19" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="D19" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="E19" s="21" t="s">
         <v>108</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B20" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B21" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
@@ -1980,49 +2124,49 @@
     </row>
     <row r="22" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B22" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>120</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>121</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B23" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="B24" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>115</v>
-      </c>
       <c r="D24" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="36"/>
+      <c r="B30" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="39"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>23</v>
@@ -2030,7 +2174,7 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>24</v>
@@ -2038,10 +2182,10 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2072,16 +2216,16 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:8">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" s="38"/>
+      <c r="G5" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1">
       <c r="B6" s="6" t="s">
@@ -2105,7 +2249,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>11</v>
@@ -2119,7 +2263,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>12</v>
@@ -2174,10 +2318,10 @@
       </c>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="41" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2239,7 +2383,7 @@
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="10">
         <v>3</v>
@@ -2247,17 +2391,17 @@
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:3">
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="43" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2294,11 +2438,11 @@
       </c>
     </row>
     <row r="37" spans="2:3">
-      <c r="B37" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>32</v>
+      <c r="B37" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="2:3">
@@ -2322,7 +2466,7 @@
         <v>20</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="2:3">
@@ -2330,18 +2474,18 @@
         <v>25</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="2:3">
-      <c r="B43" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" s="39"/>
+      <c r="B43" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="42"/>
     </row>
     <row r="44" spans="2:3">
       <c r="B44" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>23</v>
@@ -2349,7 +2493,7 @@
     </row>
     <row r="45" spans="2:3">
       <c r="B45" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>24</v>
@@ -2357,7 +2501,7 @@
     </row>
     <row r="46" spans="2:3">
       <c r="B46" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46" s="26">
         <v>2</v>
@@ -2365,7 +2509,7 @@
     </row>
     <row r="47" spans="2:3">
       <c r="B47" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" s="26">
         <v>1</v>
@@ -2386,23 +2530,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B6:C28"/>
+  <dimension ref="B6:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="31.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="40.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:3">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="44"/>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="12" t="s">
@@ -2429,17 +2575,17 @@
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="46"/>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:3">
@@ -2466,73 +2612,175 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="43"/>
-    </row>
-    <row r="21" spans="2:3">
+    <row r="20" spans="2:8">
+      <c r="B20" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="44"/>
+      <c r="F20" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" s="47"/>
+      <c r="H20" s="46"/>
+    </row>
+    <row r="21" spans="2:8">
       <c r="B21" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:3">
+      <c r="F21" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="2:8">
       <c r="B22" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
+        <v>139</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="11">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
       <c r="B23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="42"/>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="11" t="s">
+      <c r="F24" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="H24" s="29">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="11">
-        <v>12.35</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>136</v>
+      <c r="H25" s="29">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="29"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="F20:H20"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>